<commit_message>
Updated codebook from main and index manually
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="201">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="201">
   <si>
     <t>status</t>
   </si>
@@ -1113,13 +1113,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J30"/>
+  <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="C5" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="C10" sqref="C10"/>
+      <selection pane="bottomRight" activeCell="B26" sqref="A26:XFD26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1455,56 +1455,52 @@
         <v>196</v>
       </c>
     </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="C24" s="14"/>
-      <c r="D24" s="14"/>
+    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+      <c r="B24" s="16" t="s">
+        <v>172</v>
+      </c>
+      <c r="C24" s="17" t="s">
+        <v>173</v>
+      </c>
+      <c r="D24" s="17" t="s">
+        <v>190</v>
+      </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B25" s="16"/>
-    </row>
-    <row r="26" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
-      <c r="B26" s="16" t="s">
-        <v>172</v>
-      </c>
-      <c r="C26" s="17" t="s">
-        <v>173</v>
-      </c>
-      <c r="D26" s="17" t="s">
-        <v>190</v>
+      <c r="B25" s="16" t="s">
+        <v>197</v>
+      </c>
+      <c r="D25" s="17" t="s">
+        <v>198</v>
+      </c>
+      <c r="F25" s="14" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+      <c r="B26" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="F26" s="14" t="s">
+        <v>142</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.3">
       <c r="B27" s="16" t="s">
-        <v>197</v>
+        <v>154</v>
       </c>
       <c r="D27" s="17" t="s">
-        <v>198</v>
-      </c>
-    </row>
-    <row r="28" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B28" s="16"/>
-    </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B29" s="14" t="s">
-        <v>135</v>
-      </c>
-      <c r="F29" s="14" t="s">
-        <v>142</v>
-      </c>
-    </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.3">
-      <c r="B30" s="16" t="s">
-        <v>154</v>
-      </c>
-      <c r="D30" s="17" t="s">
         <v>171</v>
+      </c>
+      <c r="F27" s="14" t="s">
+        <v>172</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="C19">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B29:C1048576 B1:C4 C21:C23 B12:C18 B7:C10 B5:B6 B11 C25:C28">
+  <conditionalFormatting sqref="B26:C1048576 B1:C4 B12:C18 B7:C10 B5:B6 B11 C21:C25">
     <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2674,27 +2670,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2945,32 +2920,28 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
 </file>
 
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2987,4 +2958,29 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
Updated index and analytical dataset name
</commit_message>
<xml_diff>
--- a/i_codebooks/00_index.xlsx
+++ b/i_codebooks/00_index.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="20416"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\rosgin2\Documents\emorragie_gravi\i_codebooks\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Davide\Documents\Git repositories\Work\emorragie_gravi\i_codebooks\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{19FD8336-3399-4FB3-940B-9C3CE688AB11}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12216"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="12210" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="index" sheetId="1" r:id="rId1"/>
@@ -604,9 +605,6 @@
     <t xml:space="preserve">D3_episodes_of_treatment D3_bleeding_events </t>
   </si>
   <si>
-    <t>D4_analytic_dataset</t>
-  </si>
-  <si>
     <t>episode of bleeding including outcomes and covariates</t>
   </si>
   <si>
@@ -623,12 +621,15 @@
   </si>
   <si>
     <t>D3_dispensings_AA</t>
+  </si>
+  <si>
+    <t>D4_analytical_dataset</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -780,7 +781,7 @@
     <xf numFmtId="0" fontId="0" fillId="7" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normale" xfId="0" builtinId="0"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="2">
     <dxf>
@@ -1112,30 +1113,30 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J27"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="B1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="1" topLeftCell="E17" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="1" topLeftCell="F17" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight"/>
       <selection pane="bottomLeft"/>
-      <selection pane="bottomRight" activeCell="B26" sqref="A26:XFD26"/>
+      <selection pane="bottomRight" activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="8.88671875" style="14"/>
-    <col min="2" max="2" width="44.6640625" style="14" customWidth="1"/>
-    <col min="3" max="3" width="44.6640625" style="17" customWidth="1"/>
-    <col min="4" max="4" width="46.5546875" style="17" customWidth="1"/>
-    <col min="5" max="5" width="29.6640625" style="14" customWidth="1"/>
-    <col min="6" max="6" width="86.33203125" style="14" customWidth="1"/>
-    <col min="7" max="7" width="25.88671875" style="14" customWidth="1"/>
-    <col min="8" max="8" width="11.44140625" style="14" bestFit="1" customWidth="1"/>
-    <col min="9" max="16384" width="8.88671875" style="14"/>
+    <col min="1" max="1" width="8.85546875" style="14"/>
+    <col min="2" max="2" width="44.7109375" style="14" customWidth="1"/>
+    <col min="3" max="3" width="44.7109375" style="17" customWidth="1"/>
+    <col min="4" max="4" width="46.5703125" style="17" customWidth="1"/>
+    <col min="5" max="5" width="29.7109375" style="14" customWidth="1"/>
+    <col min="6" max="6" width="86.28515625" style="14" customWidth="1"/>
+    <col min="7" max="7" width="25.85546875" style="14" customWidth="1"/>
+    <col min="8" max="8" width="11.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="16384" width="8.85546875" style="14"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="10" t="s">
         <v>0</v>
       </c>
@@ -1167,7 +1168,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="2" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B2" s="12" t="s">
         <v>15</v>
       </c>
@@ -1183,7 +1184,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="3" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="B3" s="16" t="s">
         <v>12</v>
       </c>
@@ -1197,7 +1198,7 @@
       <c r="F3" s="14"/>
       <c r="G3" s="15"/>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4" s="14" t="s">
         <v>8</v>
       </c>
@@ -1212,7 +1213,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5" s="14" t="s">
         <v>11</v>
       </c>
@@ -1223,7 +1224,7 @@
         <v>167</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6" s="14" t="s">
         <v>14</v>
       </c>
@@ -1240,7 +1241,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="7" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B7" s="16" t="s">
         <v>138</v>
       </c>
@@ -1255,7 +1256,7 @@
       </c>
       <c r="G7" s="15"/>
     </row>
-    <row r="8" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B8" s="18" t="s">
         <v>149</v>
       </c>
@@ -1272,7 +1273,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B9" s="18" t="s">
         <v>160</v>
       </c>
@@ -1287,19 +1288,19 @@
         <v>139</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B10" s="26" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C10" s="26"/>
       <c r="D10" s="27" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="E10" s="28"/>
       <c r="F10" s="28"/>
       <c r="G10" s="28"/>
     </row>
-    <row r="11" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B11" s="16" t="s">
         <v>170</v>
       </c>
@@ -1313,7 +1314,7 @@
         <v>157</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B12" s="18" t="s">
         <v>140</v>
       </c>
@@ -1327,7 +1328,7 @@
         <v>193</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B13" s="24" t="s">
         <v>163</v>
       </c>
@@ -1337,7 +1338,7 @@
       </c>
       <c r="F13" s="16"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="B14" s="24" t="s">
         <v>178</v>
       </c>
@@ -1349,7 +1350,7 @@
       </c>
       <c r="F14" s="16"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B15" s="21" t="s">
         <v>144</v>
       </c>
@@ -1360,7 +1361,7 @@
         <v>182</v>
       </c>
     </row>
-    <row r="16" spans="1:10" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="B16" s="21" t="s">
         <v>145</v>
       </c>
@@ -1371,7 +1372,7 @@
         <v>183</v>
       </c>
     </row>
-    <row r="17" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="17" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B17" s="21" t="s">
         <v>146</v>
       </c>
@@ -1382,7 +1383,7 @@
         <v>184</v>
       </c>
     </row>
-    <row r="18" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="18" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B18" s="21" t="s">
         <v>161</v>
       </c>
@@ -1393,7 +1394,7 @@
         <v>185</v>
       </c>
     </row>
-    <row r="19" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="19" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B19" s="14" t="s">
         <v>136</v>
       </c>
@@ -1407,7 +1408,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="20" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B20" s="14" t="s">
         <v>137</v>
       </c>
@@ -1418,7 +1419,7 @@
         <v>136</v>
       </c>
     </row>
-    <row r="21" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="21" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B21" s="23" t="s">
         <v>152</v>
       </c>
@@ -1432,7 +1433,7 @@
         <v>150</v>
       </c>
     </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="22" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B22" s="23" t="s">
         <v>153</v>
       </c>
@@ -1444,18 +1445,18 @@
         <v>152</v>
       </c>
     </row>
-    <row r="23" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    <row r="23" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B23" s="14" t="s">
+        <v>200</v>
+      </c>
+      <c r="C23" s="17" t="s">
         <v>194</v>
       </c>
-      <c r="C23" s="17" t="s">
+      <c r="D23" s="17" t="s">
         <v>195</v>
       </c>
-      <c r="D23" s="17" t="s">
-        <v>196</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" ht="28.8" x14ac:dyDescent="0.3">
+    </row>
+    <row r="24" spans="2:6" ht="30" x14ac:dyDescent="0.25">
       <c r="B24" s="16" t="s">
         <v>172</v>
       </c>
@@ -1466,18 +1467,18 @@
         <v>190</v>
       </c>
     </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="25" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B25" s="16" t="s">
+        <v>196</v>
+      </c>
+      <c r="D25" s="17" t="s">
         <v>197</v>
       </c>
-      <c r="D25" s="17" t="s">
-        <v>198</v>
-      </c>
       <c r="F25" s="14" t="s">
-        <v>194</v>
-      </c>
-    </row>
-    <row r="26" spans="2:6" x14ac:dyDescent="0.3">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B26" s="14" t="s">
         <v>135</v>
       </c>
@@ -1485,7 +1486,7 @@
         <v>142</v>
       </c>
     </row>
-    <row r="27" spans="2:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="2:6" x14ac:dyDescent="0.25">
       <c r="B27" s="16" t="s">
         <v>154</v>
       </c>
@@ -1509,7 +1510,7 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:D97"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -1519,14 +1520,14 @@
       <selection pane="bottomRight" activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="26.6640625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="62.44140625" customWidth="1"/>
-    <col min="3" max="3" width="53.44140625" customWidth="1"/>
+    <col min="1" max="1" width="26.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="62.42578125" customWidth="1"/>
+    <col min="3" max="3" width="53.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:4" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="4" t="s">
         <v>22</v>
       </c>
@@ -1540,7 +1541,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>15</v>
       </c>
@@ -1551,7 +1552,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>17</v>
       </c>
@@ -1562,7 +1563,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>18</v>
       </c>
@@ -1570,7 +1571,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>18</v>
       </c>
@@ -1578,7 +1579,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>20</v>
       </c>
@@ -1589,7 +1590,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>34</v>
       </c>
@@ -1597,7 +1598,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>36</v>
       </c>
@@ -1611,7 +1612,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>36</v>
       </c>
@@ -1625,7 +1626,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>36</v>
       </c>
@@ -1639,7 +1640,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>36</v>
       </c>
@@ -1653,7 +1654,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>36</v>
       </c>
@@ -1667,7 +1668,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>36</v>
       </c>
@@ -1681,7 +1682,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>36</v>
       </c>
@@ -1695,7 +1696,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>36</v>
       </c>
@@ -1709,7 +1710,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>36</v>
       </c>
@@ -1723,7 +1724,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
         <v>36</v>
       </c>
@@ -1737,7 +1738,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
         <v>36</v>
       </c>
@@ -1751,7 +1752,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A19" s="5" t="s">
         <v>36</v>
       </c>
@@ -1765,7 +1766,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>21</v>
       </c>
@@ -1779,7 +1780,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>21</v>
       </c>
@@ -1793,7 +1794,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>21</v>
       </c>
@@ -1807,7 +1808,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1821,7 +1822,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>21</v>
       </c>
@@ -1835,7 +1836,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>21</v>
       </c>
@@ -1849,7 +1850,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>21</v>
       </c>
@@ -1863,7 +1864,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>58</v>
       </c>
@@ -1874,7 +1875,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>58</v>
       </c>
@@ -1885,7 +1886,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>58</v>
       </c>
@@ -1896,7 +1897,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>58</v>
       </c>
@@ -1907,7 +1908,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>58</v>
       </c>
@@ -1918,7 +1919,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="32" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>58</v>
       </c>
@@ -1929,7 +1930,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>58</v>
       </c>
@@ -1940,7 +1941,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>58</v>
       </c>
@@ -1951,7 +1952,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>58</v>
       </c>
@@ -1962,7 +1963,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>58</v>
       </c>
@@ -1973,7 +1974,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>58</v>
       </c>
@@ -1984,7 +1985,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>58</v>
       </c>
@@ -1995,7 +1996,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>58</v>
       </c>
@@ -2006,7 +2007,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>58</v>
       </c>
@@ -2017,7 +2018,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>58</v>
       </c>
@@ -2028,7 +2029,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>58</v>
       </c>
@@ -2039,7 +2040,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="43" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>58</v>
       </c>
@@ -2050,7 +2051,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="44" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>58</v>
       </c>
@@ -2061,7 +2062,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="45" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>58</v>
       </c>
@@ -2072,7 +2073,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="46" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>58</v>
       </c>
@@ -2083,7 +2084,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="47" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>58</v>
       </c>
@@ -2094,7 +2095,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="48" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>58</v>
       </c>
@@ -2105,7 +2106,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="49" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>58</v>
       </c>
@@ -2116,7 +2117,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="50" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>58</v>
       </c>
@@ -2127,7 +2128,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="51" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>58</v>
       </c>
@@ -2138,7 +2139,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="52" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>58</v>
       </c>
@@ -2149,7 +2150,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="53" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>58</v>
       </c>
@@ -2160,7 +2161,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="54" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>58</v>
       </c>
@@ -2171,7 +2172,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>58</v>
       </c>
@@ -2182,7 +2183,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="56" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>58</v>
       </c>
@@ -2193,7 +2194,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="57" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>58</v>
       </c>
@@ -2204,7 +2205,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="58" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>58</v>
       </c>
@@ -2215,7 +2216,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="59" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>58</v>
       </c>
@@ -2226,7 +2227,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="60" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
@@ -2237,7 +2238,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="61" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>58</v>
       </c>
@@ -2248,7 +2249,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="62" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>58</v>
       </c>
@@ -2259,7 +2260,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="63" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>58</v>
       </c>
@@ -2270,7 +2271,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="64" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>58</v>
       </c>
@@ -2281,7 +2282,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="65" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>58</v>
       </c>
@@ -2292,7 +2293,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="66" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>58</v>
       </c>
@@ -2303,7 +2304,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="67" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>58</v>
       </c>
@@ -2314,7 +2315,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="68" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>58</v>
       </c>
@@ -2325,7 +2326,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="69" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>58</v>
       </c>
@@ -2336,7 +2337,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="70" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>58</v>
       </c>
@@ -2347,7 +2348,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="71" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>58</v>
       </c>
@@ -2358,7 +2359,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="72" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>58</v>
       </c>
@@ -2369,7 +2370,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="73" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>58</v>
       </c>
@@ -2380,7 +2381,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="74" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>58</v>
       </c>
@@ -2391,7 +2392,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="75" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>58</v>
       </c>
@@ -2402,7 +2403,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="76" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>58</v>
       </c>
@@ -2413,7 +2414,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="77" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>58</v>
       </c>
@@ -2424,7 +2425,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="78" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>58</v>
       </c>
@@ -2435,7 +2436,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="79" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>58</v>
       </c>
@@ -2446,7 +2447,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>58</v>
       </c>
@@ -2457,7 +2458,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="81" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>58</v>
       </c>
@@ -2468,7 +2469,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="82" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>115</v>
       </c>
@@ -2479,7 +2480,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="83" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A83" s="8" t="s">
         <v>115</v>
       </c>
@@ -2490,7 +2491,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="85" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>120</v>
       </c>
@@ -2504,7 +2505,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="86" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>120</v>
       </c>
@@ -2518,7 +2519,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="87" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>120</v>
       </c>
@@ -2532,7 +2533,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="88" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>120</v>
       </c>
@@ -2546,7 +2547,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="89" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>120</v>
       </c>
@@ -2560,7 +2561,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="90" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>120</v>
       </c>
@@ -2574,7 +2575,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="91" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>120</v>
       </c>
@@ -2588,7 +2589,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="92" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>120</v>
       </c>
@@ -2602,7 +2603,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="93" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>120</v>
       </c>
@@ -2616,7 +2617,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="94" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>120</v>
       </c>
@@ -2630,7 +2631,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="95" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>120</v>
       </c>
@@ -2644,7 +2645,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="96" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>120</v>
       </c>
@@ -2658,7 +2659,7 @@
         <v>134</v>
       </c>
     </row>
-    <row r="97" spans="4:4" x14ac:dyDescent="0.3">
+    <row r="97" spans="4:4" x14ac:dyDescent="0.25">
       <c r="D97" t="s">
         <v>134</v>
       </c>
@@ -2670,6 +2671,27 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
+    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+  </documentManagement>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x010100051A4D12AC31714A976EFB59A015589D" ma:contentTypeVersion="17" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="8718e4a61e08f80278e3f0325a3727eb">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="8029070a-695f-410c-a424-24d0683063af" xmlns:ns3="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="8f65cc27c03321c69be19df794a0d9ee" ns2:_="" ns3:_="">
     <xsd:import namespace="8029070a-695f-410c-a424-24d0683063af"/>
@@ -2920,28 +2942,32 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
+    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <Comments xmlns="8029070a-695f-410c-a424-24d0683063af" xsi:nil="true"/>
-    <TaxCatchAll xmlns="797b3a1e-a17b-4ca2-8e72-b47fcb862c81" xsi:nil="true"/>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="8029070a-695f-410c-a424-24d0683063af">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-  </documentManagement>
-</p:properties>
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{5BC87269-1150-4B76-BCF1-DD60C8C0563E}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2958,29 +2984,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/internal/obd"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{B42E9BCA-F70C-48B3-BE7D-F5FB4AB99C58}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{57AD589C-11A6-44E8-A216-CE888FA384F2}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-    <ds:schemaRef ds:uri="797b3a1e-a17b-4ca2-8e72-b47fcb862c81"/>
-    <ds:schemaRef ds:uri="8029070a-695f-410c-a424-24d0683063af"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>